<commit_message>
fixed spelling in Test_Evaluation_Combined.xlsx
</commit_message>
<xml_diff>
--- a/evaluation/Test_Evaluation_Combined.xlsx
+++ b/evaluation/Test_Evaluation_Combined.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\IdeaProjects\zhaw-dsp-munot\evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0872BD7A-D277-4C52-A65A-EE5F58118F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A5D5DE-9373-4576-8E72-1E71E3C8AE36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t>File</t>
   </si>
@@ -110,19 +110,22 @@
     <t>3_Run_Lukas</t>
   </si>
   <si>
-    <t xml:space="preserve">Total </t>
-  </si>
-  <si>
     <t>Test_Evaluation_Nadir_Dominik.xlsx</t>
   </si>
   <si>
-    <t>Gleich</t>
-  </si>
-  <si>
-    <t>Same %</t>
-  </si>
-  <si>
-    <t>Diffrent %</t>
+    <t>total</t>
+  </si>
+  <si>
+    <t>equal</t>
+  </si>
+  <si>
+    <t>varied</t>
+  </si>
+  <si>
+    <t>equal %</t>
+  </si>
+  <si>
+    <t>varied %</t>
   </si>
 </sst>
 </file>
@@ -275,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -288,8 +291,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -578,7 +579,7 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -775,39 +776,39 @@
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>26</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="I9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9">
         <v>198</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9">
         <v>172</v>
       </c>
-      <c r="L9" s="8">
+      <c r="L9">
         <v>26</v>
       </c>
-      <c r="M9" s="9">
+      <c r="M9" s="1">
         <f>100/J9*K9</f>
         <v>86.868686868686879</v>
       </c>
-      <c r="N9" s="10">
+      <c r="N9" s="8">
         <f>100/J9*L9</f>
         <v>13.131313131313131</v>
       </c>
@@ -834,20 +835,20 @@
       <c r="I10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J10">
         <v>132</v>
       </c>
-      <c r="K10" s="8">
+      <c r="K10">
         <v>118</v>
       </c>
-      <c r="L10" s="8">
+      <c r="L10">
         <v>14</v>
       </c>
-      <c r="M10" s="9">
+      <c r="M10" s="1">
         <f t="shared" ref="M10:M12" si="4">100/J10*K10</f>
         <v>89.393939393939391</v>
       </c>
-      <c r="N10" s="10">
+      <c r="N10" s="8">
         <f t="shared" ref="N10:N12" si="5">100/J10*L10</f>
         <v>10.606060606060606</v>
       </c>
@@ -877,20 +878,20 @@
       <c r="I11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11">
         <v>132</v>
       </c>
-      <c r="K11" s="8">
+      <c r="K11">
         <v>119</v>
       </c>
-      <c r="L11" s="8">
+      <c r="L11">
         <v>13</v>
       </c>
-      <c r="M11" s="9">
+      <c r="M11" s="1">
         <f t="shared" si="4"/>
         <v>90.151515151515156</v>
       </c>
-      <c r="N11" s="10">
+      <c r="N11" s="8">
         <f t="shared" si="5"/>
         <v>9.8484848484848477</v>
       </c>
@@ -917,26 +918,26 @@
         <f t="shared" ref="F12:F13" si="8">100/B12*D12</f>
         <v>6.0606060606060606</v>
       </c>
-      <c r="I12" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="J12" s="12">
+      <c r="I12" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="10">
         <f>SUM(J9:J11)</f>
         <v>462</v>
       </c>
-      <c r="K12" s="12">
+      <c r="K12" s="10">
         <f t="shared" ref="K12:L12" si="9">SUM(K9:K11)</f>
         <v>409</v>
       </c>
-      <c r="L12" s="12">
+      <c r="L12" s="10">
         <f t="shared" si="9"/>
         <v>53</v>
       </c>
-      <c r="M12" s="13">
+      <c r="M12" s="11">
         <f t="shared" si="4"/>
         <v>88.528138528138527</v>
       </c>
-      <c r="N12" s="14">
+      <c r="N12" s="12">
         <f t="shared" si="5"/>
         <v>11.471861471861471</v>
       </c>
@@ -966,7 +967,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14">
         <v>33</v>

</xml_diff>